<commit_message>
Updated to MATLAB 2023b
</commit_message>
<xml_diff>
--- a/temp_data.xlsx
+++ b/temp_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\0_Projects\0.Bachelor Theses_MOC Nozzle Design\MOC CODE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\MOC-2D-Nozzle-Design-Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE7D086-8011-4A85-975B-4844A8E7AE7E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B5C75D7-D4D2-41AC-B703-7E242D954FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="7890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5670" yWindow="3510" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -343,7 +343,10 @@
       <selection sqref="A1:B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="7"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
@@ -355,122 +358,122 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1.1948490676750452</v>
+        <v>1.3760406834250329</v>
       </c>
       <c r="B2">
-        <v>1.2703715138776879</v>
+        <v>1.4407606868944756</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1.6719928171950471</v>
+        <v>2.033274321331886</v>
       </c>
       <c r="B3">
-        <v>1.3706683346835644</v>
+        <v>1.635890667751646</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1.917925931917783</v>
+        <v>2.3907382043656482</v>
       </c>
       <c r="B4">
-        <v>1.4184353256557771</v>
+        <v>1.7337558547909908</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2.1440521925713605</v>
+        <v>2.7372971564433803</v>
       </c>
       <c r="B5">
-        <v>1.4587643958325736</v>
+        <v>1.8207165240049576</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2.3626221570476669</v>
+        <v>3.0882649800088</v>
       </c>
       <c r="B6">
-        <v>1.4942938792848621</v>
+        <v>1.9008493403852094</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2.5794719212044903</v>
+        <v>3.4517297632007469</v>
       </c>
       <c r="B7">
-        <v>1.5261360114586853</v>
+        <v>1.9756986257760056</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2.7980040440192027</v>
+        <v>3.8331534197834287</v>
       </c>
       <c r="B8">
-        <v>1.5548064620447037</v>
+        <v>2.0457822230274285</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>3.0204975517098953</v>
+        <v>4.236896125644944</v>
       </c>
       <c r="B9">
-        <v>1.5805299279522262</v>
+        <v>2.1110776111208867</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>3.2486483969144757</v>
+        <v>4.6668580954829482</v>
       </c>
       <c r="B10">
-        <v>1.6033652089609989</v>
+        <v>2.1712121334138463</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>3.4838278925351478</v>
+        <v>5.126800411866272</v>
       </c>
       <c r="B11">
-        <v>1.6232637971797412</v>
+        <v>2.2255429706600935</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>3.7272202416085172</v>
+        <v>5.6205306047007726</v>
       </c>
       <c r="B12">
-        <v>1.6400997475703241</v>
+        <v>2.273187971651319</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>3.9799021293818928</v>
+        <v>6.1520257814507477</v>
       </c>
       <c r="B13">
-        <v>1.6536856062886707</v>
+        <v>2.3130309116000372</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>4.242892148014711</v>
+        <v>6.7255257280586287</v>
       </c>
       <c r="B14">
-        <v>1.663780910738242</v>
+        <v>2.3437112142351899</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>4.5171834858809827</v>
+        <v>7.3456120296450624</v>
       </c>
       <c r="B15">
-        <v>1.6700964006544659</v>
+        <v>2.3636025870620045</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>4.803766873072588</v>
+        <v>8.0172819828917472</v>
       </c>
       <c r="B16">
-        <v>1.6722955590280586</v>
+        <v>2.3707824297215985</v>
       </c>
     </row>
   </sheetData>

</xml_diff>